<commit_message>
search delete view testing
</commit_message>
<xml_diff>
--- a/src/components/Student_details.xlsx
+++ b/src/components/Student_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arun\MERN\Intership\LinkUrCodes-Event-App-FrontEnd\src\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E9C607-8969-4BCB-A8D0-30C184C187CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50EA957-39EB-491D-AC38-D81DD284FCCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A984402D-1A8C-4151-94EC-7BECCC5AFD9A}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{A984402D-1A8C-4151-94EC-7BECCC5AFD9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>student_name</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>event_id</t>
-  </si>
-  <si>
-    <t>student_college_id</t>
   </si>
   <si>
     <t>student_admno</t>
@@ -455,7 +452,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="A2:G4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,10 +473,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -487,9 +484,7 @@
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E2" s="2"/>

</xml_diff>

<commit_message>
view and add student in college correctedd
</commit_message>
<xml_diff>
--- a/src/components/Student_details.xlsx
+++ b/src/components/Student_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arun\MERN\Intership\LinkUrCodes-Event-App-FrontEnd\src\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50EA957-39EB-491D-AC38-D81DD284FCCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297E018B-08A2-4743-999B-685C97E07482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{A984402D-1A8C-4151-94EC-7BECCC5AFD9A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>student_name</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>student_email</t>
-  </si>
-  <si>
-    <t>event_id</t>
   </si>
   <si>
     <t>student_admno</t>
@@ -452,7 +449,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F3" sqref="F1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,17 +470,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>